<commit_message>
Aktualisierung der Kürzel in der Hoffnung auf Behebung des Problems der fehlschagenden Klicks
</commit_message>
<xml_diff>
--- a/Archiv.xlsx
+++ b/Archiv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ec4a8a11e8d582b/Desktop/Archiv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{8A0600A5-B62D-4D09-9E5B-AEDD842D3B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1936082E-422A-40FC-BE82-1CB15E7DDC1E}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{8A0600A5-B62D-4D09-9E5B-AEDD842D3B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BE767EF-C478-4023-81A5-21B46B000E39}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F80365CE-59B1-456A-8E15-81802F42A1A9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
   <si>
     <t>Titel</t>
   </si>
@@ -1365,6 +1365,9 @@
   </si>
   <si>
     <t>Gegenstand dieses Berichts sind Erkenntnisse bezüglich eines Umweltvergehens, das vom Betreiber der Chemunich-Fabrik in der Nähe von München, Hagen Achleitner, begangen wurde. Meine Untersuchungen ergaben Hinweise, dass die Fabrik kontaminiertes Wasser illegal in einen Zufluss der Isar leitet, wodurch einheimische Arten, insbesondere die Bayerische Zwergdeckelschnecke, gefährdet sind. Hintergrund: Die Bayerische Zwergdeckelschnecke ist eine endemische Art, die ausschließlich in der Region München vorkommt. Diese Spezies hat eine bedeutende ökologische Rolle im Ökosystem der Isar und aufgrund des geschilderten Umstandes nunmehr als vom Aussterben bedroht eingestuft werden. Haupterkenntnisse: Überwachungsmaßnahmen haben ergeben, dass Chemunich regelmäßig ungewöhnliche Abwassermengen in einen nahegelegenen Wasserlauf einleitet. Analytische Tests des Wassers zeigten einen hohen Gehalt an verschiedenen Chemikalien, die in der Fabrik verwendet werden. Unterirdische Rohrleitungen, die von der Fabrik wegführen, wurden identifiziert und es besteht der Verdacht, dass diese zur geheimen Ableitung von Abwässern genutzt werden. Einige ehemalige Mitarbeiter der Fabrik bestätigten unter der Bedingung der Anonymität, dass sie von der illegalen Entsorgung von Abwässern gewusst haben. Schlussfolgerungen: Es besteht ein dringender Verdacht, dass die Chemunich-Fabrik unter der Leitung von Hagen Achleitner gegen Umweltschutzgesetze verstößt, indem sie kontaminiertes Abwasser in die Isar leitet. Das unmittelbare Resultat dieses Vergehens ist die Gefährdung der Bayerischen Zwergdeckelschnecke und potenziell anderer Tier- und Pflanzenarten in diesem Gebiet. Wichtige Anmerkung: Zum Zwecke meiner Recherche habe ich mir von meinem EDV-Dienstleister einen Zugang zu Hagen Achleitners E-Mail-Postfach legen lassen. Unter diesem kann seine Korrespondenz nachgelesen werden. Eventuell erhalte ich dort weitere Hinweise. Der Zugang ist hier zu erreichen: https://me-qr.com/1TUcWHQ7</t>
+  </si>
+  <si>
+    <t>Kürzel</t>
   </si>
 </sst>
 </file>
@@ -1425,11 +1428,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1748,772 +1752,1054 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE33CEFD-DBA8-4D6E-97C7-B35BC24E17BF}">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A58" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>4689</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>4690</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>4691</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>4692</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <v>4693</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>4694</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>4695</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>4696</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>4697</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>4698</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>4699</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>4700</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <v>4701</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>4702</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>4703</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>4704</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>4705</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>4706</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>4707</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>4708</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>4709</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>4710</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <v>4711</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <v>4712</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A26" s="4">
+        <v>4713</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
+        <v>4714</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
+        <v>4715</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A29" s="4">
+        <v>4716</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A30" s="4">
+        <v>4717</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A31" s="4">
+        <v>4718</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A32" s="4">
+        <v>4719</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A33" s="4">
+        <v>4720</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A34" s="4">
+        <v>4721</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A35" s="4">
+        <v>4722</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A36" s="4">
+        <v>4723</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A37" s="4">
+        <v>4724</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A38" s="4">
+        <v>4725</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A39" s="4">
+        <v>4726</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A40" s="4">
+        <v>4727</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A41" s="4">
+        <v>4728</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A42" s="4">
+        <v>4729</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A43" s="4">
+        <v>4730</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A44" s="4">
+        <v>4731</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A45" s="4">
+        <v>4732</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A46" s="4">
+        <v>4733</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A47" s="4">
+        <v>4734</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A48" s="4">
+        <v>4735</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A49" s="4">
+        <v>4736</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A50" s="4">
+        <v>4737</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A51" s="4">
+        <v>4738</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A52" s="4">
+        <v>4739</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A53" s="4">
+        <v>4740</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A54" s="4">
+        <v>4741</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A55" s="4">
+        <v>4742</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A56" s="4">
+        <v>4743</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A57" s="4">
+        <v>4744</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A58" s="4">
+        <v>4745</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A59" s="4">
+        <v>4746</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A60" s="4">
+        <v>4747</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A61" s="4">
+        <v>4748</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A62" s="3" t="s">
+    <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A62" s="4">
+        <v>4749</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A63" s="4">
+        <v>4750</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A64" s="4">
+        <v>4751</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A65" s="3" t="s">
+    <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A65" s="4">
+        <v>4752</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="4">
+        <v>4753</v>
+      </c>
+      <c r="B66" t="s">
         <v>132</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="4">
+        <v>4754</v>
+      </c>
+      <c r="B67" t="s">
         <v>134</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="4">
+        <v>4755</v>
+      </c>
+      <c r="B68" t="s">
         <v>136</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="4">
+        <v>4756</v>
+      </c>
+      <c r="B69" t="s">
         <v>138</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="4">
+        <v>4757</v>
+      </c>
+      <c r="B70" t="s">
         <v>140</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="4">
+        <v>4758</v>
+      </c>
+      <c r="B71" t="s">
         <v>142</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="4">
+        <v>4759</v>
+      </c>
+      <c r="B72" t="s">
         <v>144</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="4">
+        <v>4760</v>
+      </c>
+      <c r="B73" t="s">
         <v>146</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="4">
+        <v>4761</v>
+      </c>
+      <c r="B74" t="s">
         <v>148</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="4">
+        <v>4762</v>
+      </c>
+      <c r="B75" t="s">
         <v>150</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="4">
+        <v>4763</v>
+      </c>
+      <c r="B76" t="s">
         <v>152</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="4">
+        <v>4764</v>
+      </c>
+      <c r="B77" t="s">
         <v>154</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="4">
+        <v>4765</v>
+      </c>
+      <c r="B78" t="s">
         <v>156</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="4">
+        <v>4766</v>
+      </c>
+      <c r="B79" t="s">
         <v>158</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="4">
+        <v>4767</v>
+      </c>
+      <c r="B80" t="s">
         <v>160</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="4">
+        <v>4768</v>
+      </c>
+      <c r="B81" t="s">
         <v>162</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="4">
+        <v>4769</v>
+      </c>
+      <c r="B82" t="s">
         <v>164</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="4">
+        <v>4770</v>
+      </c>
+      <c r="B83" t="s">
         <v>166</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="4">
+        <v>4771</v>
+      </c>
+      <c r="B84" t="s">
         <v>168</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="4">
+        <v>4772</v>
+      </c>
+      <c r="B85" t="s">
         <v>170</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="4">
+        <v>4773</v>
+      </c>
+      <c r="B86" t="s">
         <v>172</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="4">
+        <v>4774</v>
+      </c>
+      <c r="B87" t="s">
         <v>174</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="4">
+        <v>4775</v>
+      </c>
+      <c r="B88" t="s">
         <v>176</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="4">
+        <v>4776</v>
+      </c>
+      <c r="B89" t="s">
         <v>178</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="4">
+        <v>4777</v>
+      </c>
+      <c r="B90" t="s">
         <v>180</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="4">
+        <v>4778</v>
+      </c>
+      <c r="B91" t="s">
         <v>182</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="4">
+        <v>4779</v>
+      </c>
+      <c r="B92" t="s">
         <v>184</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="4">
+        <v>4780</v>
+      </c>
+      <c r="B93" t="s">
         <v>186</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="4">
+        <v>4781</v>
+      </c>
+      <c r="B94" t="s">
         <v>188</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>189</v>
       </c>
     </row>

</xml_diff>